<commit_message>
Fixed account receivable issue
</commit_message>
<xml_diff>
--- a/PopuliQB_Tool/QB- Item List.xlsx
+++ b/PopuliQB_Tool/QB- Item List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Upwork\QueensCounsulting\PopuliQB1\PopuliQB_Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2-JOB\Upwork\QueensCounsulting\PopuliQB1\PopuliQB_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B51A338-E55A-435E-A98C-1CBA01A751D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" activeTab="1" xr2:uid="{D1EC46F2-DFE4-4AD9-84B0-06E54D97CEF4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Item List- Invoice" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Item List- Credit memo'!$A$1:$A$164</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Item List- Invoice'!$A$1:$B$39</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="244">
   <si>
     <t>414220 ·: Student Tech Fees- MSP</t>
   </si>
@@ -759,12 +758,15 @@
   </si>
   <si>
     <t>MOU MSC St. Paul's Outreach 25%</t>
+  </si>
+  <si>
+    <t>MSP- FT (Summer) 0.00-3.00 credits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1124,12 +1126,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5315B542-CA34-4B58-8AC4-D11D579A4569}">
-  <dimension ref="A1:B42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,6 +1476,14 @@
         <v>53</v>
       </c>
     </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>243</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1481,17 +1491,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BDCA46-2904-4506-8B07-72BBEE74628B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="1" max="1" width="66.140625" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2800,7 +2810,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A164" xr:uid="{4F62D15F-756B-49BC-BF70-D80BD1762776}"/>
+  <autoFilter ref="A1:A164"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>